<commit_message>
Making changes to data wrangling steps
</commit_message>
<xml_diff>
--- a/Processed_Data/Sus_Env_Processed.xlsx
+++ b/Processed_Data/Sus_Env_Processed.xlsx
@@ -351,7 +351,7 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <dimension ref="A1:E177"/>
+  <dimension ref="A1:E133"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0"/>
   </sheetViews>
@@ -1209,17 +1209,17 @@
     <row r="35">
       <c r="A35" t="inlineStr">
         <is>
-          <t>China</t>
+          <t>United States</t>
         </is>
       </c>
       <c r="B35" t="inlineStr">
         <is>
-          <t>CHN</t>
+          <t>USA</t>
         </is>
       </c>
       <c r="C35" t="inlineStr">
         <is>
-          <t>Cook</t>
+          <t>PM</t>
         </is>
       </c>
       <c r="D35" t="inlineStr">
@@ -1228,23 +1228,23 @@
         </is>
       </c>
       <c r="E35">
-        <v>58.1</v>
+        <v>9.221851825</v>
       </c>
     </row>
     <row r="36">
       <c r="A36" t="inlineStr">
         <is>
-          <t>China</t>
+          <t>United States</t>
         </is>
       </c>
       <c r="B36" t="inlineStr">
         <is>
-          <t>CHN</t>
+          <t>USA</t>
         </is>
       </c>
       <c r="C36" t="inlineStr">
         <is>
-          <t>Cook</t>
+          <t>PM</t>
         </is>
       </c>
       <c r="D36" t="inlineStr">
@@ -1253,23 +1253,23 @@
         </is>
       </c>
       <c r="E36">
-        <v>60.7</v>
+        <v>9.262992540000001</v>
       </c>
     </row>
     <row r="37">
       <c r="A37" t="inlineStr">
         <is>
-          <t>China</t>
+          <t>United States</t>
         </is>
       </c>
       <c r="B37" t="inlineStr">
         <is>
-          <t>CHN</t>
+          <t>USA</t>
         </is>
       </c>
       <c r="C37" t="inlineStr">
         <is>
-          <t>Cook</t>
+          <t>PM</t>
         </is>
       </c>
       <c r="D37" t="inlineStr">
@@ -1278,23 +1278,23 @@
         </is>
       </c>
       <c r="E37">
-        <v>63.2</v>
+        <v>8.869988146000001</v>
       </c>
     </row>
     <row r="38">
       <c r="A38" t="inlineStr">
         <is>
-          <t>China</t>
+          <t>United States</t>
         </is>
       </c>
       <c r="B38" t="inlineStr">
         <is>
-          <t>CHN</t>
+          <t>USA</t>
         </is>
       </c>
       <c r="C38" t="inlineStr">
         <is>
-          <t>Cook</t>
+          <t>PM</t>
         </is>
       </c>
       <c r="D38" t="inlineStr">
@@ -1303,23 +1303,23 @@
         </is>
       </c>
       <c r="E38">
-        <v>65.59999999999999</v>
+        <v>8.641628969999999</v>
       </c>
     </row>
     <row r="39">
       <c r="A39" t="inlineStr">
         <is>
-          <t>China</t>
+          <t>United States</t>
         </is>
       </c>
       <c r="B39" t="inlineStr">
         <is>
-          <t>CHN</t>
+          <t>USA</t>
         </is>
       </c>
       <c r="C39" t="inlineStr">
         <is>
-          <t>Cook</t>
+          <t>PM</t>
         </is>
       </c>
       <c r="D39" t="inlineStr">
@@ -1328,23 +1328,23 @@
         </is>
       </c>
       <c r="E39">
-        <v>68.2</v>
+        <v>8.433002377999999</v>
       </c>
     </row>
     <row r="40">
       <c r="A40" t="inlineStr">
         <is>
-          <t>China</t>
+          <t>United States</t>
         </is>
       </c>
       <c r="B40" t="inlineStr">
         <is>
-          <t>CHN</t>
+          <t>USA</t>
         </is>
       </c>
       <c r="C40" t="inlineStr">
         <is>
-          <t>Cook</t>
+          <t>PM</t>
         </is>
       </c>
       <c r="D40" t="inlineStr">
@@ -1353,23 +1353,23 @@
         </is>
       </c>
       <c r="E40">
-        <v>70.59999999999999</v>
+        <v>8.163752791</v>
       </c>
     </row>
     <row r="41">
       <c r="A41" t="inlineStr">
         <is>
-          <t>China</t>
+          <t>United States</t>
         </is>
       </c>
       <c r="B41" t="inlineStr">
         <is>
-          <t>CHN</t>
+          <t>USA</t>
         </is>
       </c>
       <c r="C41" t="inlineStr">
         <is>
-          <t>Cook</t>
+          <t>PM</t>
         </is>
       </c>
       <c r="D41" t="inlineStr">
@@ -1378,23 +1378,23 @@
         </is>
       </c>
       <c r="E41">
-        <v>73.09999999999999</v>
+        <v>7.378939412</v>
       </c>
     </row>
     <row r="42">
       <c r="A42" t="inlineStr">
         <is>
-          <t>China</t>
+          <t>United States</t>
         </is>
       </c>
       <c r="B42" t="inlineStr">
         <is>
-          <t>CHN</t>
+          <t>USA</t>
         </is>
       </c>
       <c r="C42" t="inlineStr">
         <is>
-          <t>Cook</t>
+          <t>PM</t>
         </is>
       </c>
       <c r="D42" t="inlineStr">
@@ -1403,23 +1403,23 @@
         </is>
       </c>
       <c r="E42">
-        <v>75.40000000000001</v>
+        <v>7.74468451</v>
       </c>
     </row>
     <row r="43">
       <c r="A43" t="inlineStr">
         <is>
-          <t>China</t>
+          <t>United States</t>
         </is>
       </c>
       <c r="B43" t="inlineStr">
         <is>
-          <t>CHN</t>
+          <t>USA</t>
         </is>
       </c>
       <c r="C43" t="inlineStr">
         <is>
-          <t>Cook</t>
+          <t>PM</t>
         </is>
       </c>
       <c r="D43" t="inlineStr">
@@ -1428,23 +1428,23 @@
         </is>
       </c>
       <c r="E43">
-        <v>77.59999999999999</v>
+        <v>7.775115257</v>
       </c>
     </row>
     <row r="44">
       <c r="A44" t="inlineStr">
         <is>
-          <t>China</t>
+          <t>United States</t>
         </is>
       </c>
       <c r="B44" t="inlineStr">
         <is>
-          <t>CHN</t>
+          <t>USA</t>
         </is>
       </c>
       <c r="C44" t="inlineStr">
         <is>
-          <t>Cook</t>
+          <t>PM</t>
         </is>
       </c>
       <c r="D44" t="inlineStr">
@@ -1453,32 +1453,29 @@
         </is>
       </c>
       <c r="E44">
-        <v>79.40000000000001</v>
+        <v>7.663692516</v>
       </c>
     </row>
     <row r="45">
       <c r="A45" t="inlineStr">
         <is>
-          <t>China</t>
+          <t>United States</t>
         </is>
       </c>
       <c r="B45" t="inlineStr">
         <is>
-          <t>CHN</t>
+          <t>USA</t>
         </is>
       </c>
       <c r="C45" t="inlineStr">
         <is>
-          <t>Cook</t>
+          <t>PM</t>
         </is>
       </c>
       <c r="D45" t="inlineStr">
         <is>
           <t>2020</t>
         </is>
-      </c>
-      <c r="E45">
-        <v>81.40000000000001</v>
       </c>
     </row>
     <row r="46">
@@ -1494,7 +1491,7 @@
       </c>
       <c r="C46" t="inlineStr">
         <is>
-          <t>PM</t>
+          <t>CO2</t>
         </is>
       </c>
       <c r="D46" t="inlineStr">
@@ -1503,7 +1500,7 @@
         </is>
       </c>
       <c r="E46">
-        <v>9.221851825</v>
+        <v>17.4317369879177</v>
       </c>
     </row>
     <row r="47">
@@ -1519,7 +1516,7 @@
       </c>
       <c r="C47" t="inlineStr">
         <is>
-          <t>PM</t>
+          <t>CO2</t>
         </is>
       </c>
       <c r="D47" t="inlineStr">
@@ -1528,7 +1525,7 @@
         </is>
       </c>
       <c r="E47">
-        <v>9.262992540000001</v>
+        <v>16.604189616843</v>
       </c>
     </row>
     <row r="48">
@@ -1544,7 +1541,7 @@
       </c>
       <c r="C48" t="inlineStr">
         <is>
-          <t>PM</t>
+          <t>CO2</t>
         </is>
       </c>
       <c r="D48" t="inlineStr">
@@ -1553,7 +1550,7 @@
         </is>
       </c>
       <c r="E48">
-        <v>8.869988146000001</v>
+        <v>15.789760151839</v>
       </c>
     </row>
     <row r="49">
@@ -1569,7 +1566,7 @@
       </c>
       <c r="C49" t="inlineStr">
         <is>
-          <t>PM</t>
+          <t>CO2</t>
         </is>
       </c>
       <c r="D49" t="inlineStr">
@@ -1578,7 +1575,7 @@
         </is>
       </c>
       <c r="E49">
-        <v>8.641628969999999</v>
+        <v>16.1111752638496</v>
       </c>
     </row>
     <row r="50">
@@ -1594,7 +1591,7 @@
       </c>
       <c r="C50" t="inlineStr">
         <is>
-          <t>PM</t>
+          <t>CO2</t>
         </is>
       </c>
       <c r="D50" t="inlineStr">
@@ -1603,7 +1600,7 @@
         </is>
       </c>
       <c r="E50">
-        <v>8.433002377999999</v>
+        <v>16.0409167568247</v>
       </c>
     </row>
     <row r="51">
@@ -1619,7 +1616,7 @@
       </c>
       <c r="C51" t="inlineStr">
         <is>
-          <t>PM</t>
+          <t>CO2</t>
         </is>
       </c>
       <c r="D51" t="inlineStr">
@@ -1628,7 +1625,7 @@
         </is>
       </c>
       <c r="E51">
-        <v>8.163752791</v>
+        <v>15.5600154435853</v>
       </c>
     </row>
     <row r="52">
@@ -1644,7 +1641,7 @@
       </c>
       <c r="C52" t="inlineStr">
         <is>
-          <t>PM</t>
+          <t>CO2</t>
         </is>
       </c>
       <c r="D52" t="inlineStr">
@@ -1653,7 +1650,7 @@
         </is>
       </c>
       <c r="E52">
-        <v>7.378939412</v>
+        <v>15.1498827249693</v>
       </c>
     </row>
     <row r="53">
@@ -1669,7 +1666,7 @@
       </c>
       <c r="C53" t="inlineStr">
         <is>
-          <t>PM</t>
+          <t>CO2</t>
         </is>
       </c>
       <c r="D53" t="inlineStr">
@@ -1678,7 +1675,7 @@
         </is>
       </c>
       <c r="E53">
-        <v>7.74468451</v>
+        <v>14.8232454359428</v>
       </c>
     </row>
     <row r="54">
@@ -1694,7 +1691,7 @@
       </c>
       <c r="C54" t="inlineStr">
         <is>
-          <t>PM</t>
+          <t>CO2</t>
         </is>
       </c>
       <c r="D54" t="inlineStr">
@@ -1703,7 +1700,7 @@
         </is>
       </c>
       <c r="E54">
-        <v>7.775115257</v>
+        <v>15.2225180998504</v>
       </c>
     </row>
     <row r="55">
@@ -1719,7 +1716,7 @@
       </c>
       <c r="C55" t="inlineStr">
         <is>
-          <t>PM</t>
+          <t>CO2</t>
         </is>
       </c>
       <c r="D55" t="inlineStr">
@@ -1728,7 +1725,7 @@
         </is>
       </c>
       <c r="E55">
-        <v>7.663692516</v>
+        <v>14.6733807134556</v>
       </c>
     </row>
     <row r="56">
@@ -1744,13 +1741,16 @@
       </c>
       <c r="C56" t="inlineStr">
         <is>
-          <t>PM</t>
+          <t>CO2</t>
         </is>
       </c>
       <c r="D56" t="inlineStr">
         <is>
           <t>2020</t>
         </is>
+      </c>
+      <c r="E56">
+        <v>13.0328279519898</v>
       </c>
     </row>
     <row r="57">
@@ -1766,7 +1766,7 @@
       </c>
       <c r="C57" t="inlineStr">
         <is>
-          <t>CO2</t>
+          <t>Renew</t>
         </is>
       </c>
       <c r="D57" t="inlineStr">
@@ -1775,7 +1775,7 @@
         </is>
       </c>
       <c r="E57">
-        <v>17.4317369879177</v>
+        <v>7.44</v>
       </c>
     </row>
     <row r="58">
@@ -1791,7 +1791,7 @@
       </c>
       <c r="C58" t="inlineStr">
         <is>
-          <t>CO2</t>
+          <t>Renew</t>
         </is>
       </c>
       <c r="D58" t="inlineStr">
@@ -1800,7 +1800,7 @@
         </is>
       </c>
       <c r="E58">
-        <v>16.604189616843</v>
+        <v>8.359999999999999</v>
       </c>
     </row>
     <row r="59">
@@ -1816,7 +1816,7 @@
       </c>
       <c r="C59" t="inlineStr">
         <is>
-          <t>CO2</t>
+          <t>Renew</t>
         </is>
       </c>
       <c r="D59" t="inlineStr">
@@ -1825,7 +1825,7 @@
         </is>
       </c>
       <c r="E59">
-        <v>15.789760151839</v>
+        <v>8.73</v>
       </c>
     </row>
     <row r="60">
@@ -1841,7 +1841,7 @@
       </c>
       <c r="C60" t="inlineStr">
         <is>
-          <t>CO2</t>
+          <t>Renew</t>
         </is>
       </c>
       <c r="D60" t="inlineStr">
@@ -1850,7 +1850,7 @@
         </is>
       </c>
       <c r="E60">
-        <v>16.1111752638496</v>
+        <v>9.08</v>
       </c>
     </row>
     <row r="61">
@@ -1866,7 +1866,7 @@
       </c>
       <c r="C61" t="inlineStr">
         <is>
-          <t>CO2</t>
+          <t>Renew</t>
         </is>
       </c>
       <c r="D61" t="inlineStr">
@@ -1875,7 +1875,7 @@
         </is>
       </c>
       <c r="E61">
-        <v>16.0409167568247</v>
+        <v>9.220000000000001</v>
       </c>
     </row>
     <row r="62">
@@ -1891,7 +1891,7 @@
       </c>
       <c r="C62" t="inlineStr">
         <is>
-          <t>CO2</t>
+          <t>Renew</t>
         </is>
       </c>
       <c r="D62" t="inlineStr">
@@ -1900,7 +1900,7 @@
         </is>
       </c>
       <c r="E62">
-        <v>15.5600154435853</v>
+        <v>9.029999999999999</v>
       </c>
     </row>
     <row r="63">
@@ -1916,7 +1916,7 @@
       </c>
       <c r="C63" t="inlineStr">
         <is>
-          <t>CO2</t>
+          <t>Renew</t>
         </is>
       </c>
       <c r="D63" t="inlineStr">
@@ -1925,7 +1925,7 @@
         </is>
       </c>
       <c r="E63">
-        <v>15.1498827249693</v>
+        <v>9.460000000000001</v>
       </c>
     </row>
     <row r="64">
@@ -1941,7 +1941,7 @@
       </c>
       <c r="C64" t="inlineStr">
         <is>
-          <t>CO2</t>
+          <t>Renew</t>
         </is>
       </c>
       <c r="D64" t="inlineStr">
@@ -1950,7 +1950,7 @@
         </is>
       </c>
       <c r="E64">
-        <v>14.8232454359428</v>
+        <v>9.92</v>
       </c>
     </row>
     <row r="65">
@@ -1966,7 +1966,7 @@
       </c>
       <c r="C65" t="inlineStr">
         <is>
-          <t>CO2</t>
+          <t>Renew</t>
         </is>
       </c>
       <c r="D65" t="inlineStr">
@@ -1975,7 +1975,7 @@
         </is>
       </c>
       <c r="E65">
-        <v>15.2225180998504</v>
+        <v>10.12</v>
       </c>
     </row>
     <row r="66">
@@ -1991,7 +1991,7 @@
       </c>
       <c r="C66" t="inlineStr">
         <is>
-          <t>CO2</t>
+          <t>Renew</t>
         </is>
       </c>
       <c r="D66" t="inlineStr">
@@ -2000,7 +2000,7 @@
         </is>
       </c>
       <c r="E66">
-        <v>14.6733807134556</v>
+        <v>10.42</v>
       </c>
     </row>
     <row r="67">
@@ -2016,7 +2016,7 @@
       </c>
       <c r="C67" t="inlineStr">
         <is>
-          <t>CO2</t>
+          <t>Renew</t>
         </is>
       </c>
       <c r="D67" t="inlineStr">
@@ -2025,23 +2025,23 @@
         </is>
       </c>
       <c r="E67">
-        <v>13.0328279519898</v>
+        <v>11.16</v>
       </c>
     </row>
     <row r="68">
       <c r="A68" t="inlineStr">
         <is>
-          <t>United States</t>
+          <t>Colombia</t>
         </is>
       </c>
       <c r="B68" t="inlineStr">
         <is>
-          <t>USA</t>
+          <t>COL</t>
         </is>
       </c>
       <c r="C68" t="inlineStr">
         <is>
-          <t>Renew</t>
+          <t>PM</t>
         </is>
       </c>
       <c r="D68" t="inlineStr">
@@ -2050,23 +2050,23 @@
         </is>
       </c>
       <c r="E68">
-        <v>7.44</v>
+        <v>25.0816067</v>
       </c>
     </row>
     <row r="69">
       <c r="A69" t="inlineStr">
         <is>
-          <t>United States</t>
+          <t>Colombia</t>
         </is>
       </c>
       <c r="B69" t="inlineStr">
         <is>
-          <t>USA</t>
+          <t>COL</t>
         </is>
       </c>
       <c r="C69" t="inlineStr">
         <is>
-          <t>Renew</t>
+          <t>PM</t>
         </is>
       </c>
       <c r="D69" t="inlineStr">
@@ -2075,23 +2075,23 @@
         </is>
       </c>
       <c r="E69">
-        <v>8.359999999999999</v>
+        <v>25.94720366</v>
       </c>
     </row>
     <row r="70">
       <c r="A70" t="inlineStr">
         <is>
-          <t>United States</t>
+          <t>Colombia</t>
         </is>
       </c>
       <c r="B70" t="inlineStr">
         <is>
-          <t>USA</t>
+          <t>COL</t>
         </is>
       </c>
       <c r="C70" t="inlineStr">
         <is>
-          <t>Renew</t>
+          <t>PM</t>
         </is>
       </c>
       <c r="D70" t="inlineStr">
@@ -2100,23 +2100,23 @@
         </is>
       </c>
       <c r="E70">
-        <v>8.73</v>
+        <v>23.4265212</v>
       </c>
     </row>
     <row r="71">
       <c r="A71" t="inlineStr">
         <is>
-          <t>United States</t>
+          <t>Colombia</t>
         </is>
       </c>
       <c r="B71" t="inlineStr">
         <is>
-          <t>USA</t>
+          <t>COL</t>
         </is>
       </c>
       <c r="C71" t="inlineStr">
         <is>
-          <t>Renew</t>
+          <t>PM</t>
         </is>
       </c>
       <c r="D71" t="inlineStr">
@@ -2125,23 +2125,23 @@
         </is>
       </c>
       <c r="E71">
-        <v>9.08</v>
+        <v>24.2848162</v>
       </c>
     </row>
     <row r="72">
       <c r="A72" t="inlineStr">
         <is>
-          <t>United States</t>
+          <t>Colombia</t>
         </is>
       </c>
       <c r="B72" t="inlineStr">
         <is>
-          <t>USA</t>
+          <t>COL</t>
         </is>
       </c>
       <c r="C72" t="inlineStr">
         <is>
-          <t>Renew</t>
+          <t>PM</t>
         </is>
       </c>
       <c r="D72" t="inlineStr">
@@ -2150,23 +2150,23 @@
         </is>
       </c>
       <c r="E72">
-        <v>9.220000000000001</v>
+        <v>23.85881131</v>
       </c>
     </row>
     <row r="73">
       <c r="A73" t="inlineStr">
         <is>
-          <t>United States</t>
+          <t>Colombia</t>
         </is>
       </c>
       <c r="B73" t="inlineStr">
         <is>
-          <t>USA</t>
+          <t>COL</t>
         </is>
       </c>
       <c r="C73" t="inlineStr">
         <is>
-          <t>Renew</t>
+          <t>PM</t>
         </is>
       </c>
       <c r="D73" t="inlineStr">
@@ -2175,23 +2175,23 @@
         </is>
       </c>
       <c r="E73">
-        <v>9.029999999999999</v>
+        <v>22.92043409</v>
       </c>
     </row>
     <row r="74">
       <c r="A74" t="inlineStr">
         <is>
-          <t>United States</t>
+          <t>Colombia</t>
         </is>
       </c>
       <c r="B74" t="inlineStr">
         <is>
-          <t>USA</t>
+          <t>COL</t>
         </is>
       </c>
       <c r="C74" t="inlineStr">
         <is>
-          <t>Renew</t>
+          <t>PM</t>
         </is>
       </c>
       <c r="D74" t="inlineStr">
@@ -2200,23 +2200,23 @@
         </is>
       </c>
       <c r="E74">
-        <v>9.460000000000001</v>
+        <v>22.72386043</v>
       </c>
     </row>
     <row r="75">
       <c r="A75" t="inlineStr">
         <is>
-          <t>United States</t>
+          <t>Colombia</t>
         </is>
       </c>
       <c r="B75" t="inlineStr">
         <is>
-          <t>USA</t>
+          <t>COL</t>
         </is>
       </c>
       <c r="C75" t="inlineStr">
         <is>
-          <t>Renew</t>
+          <t>PM</t>
         </is>
       </c>
       <c r="D75" t="inlineStr">
@@ -2225,23 +2225,23 @@
         </is>
       </c>
       <c r="E75">
-        <v>9.92</v>
+        <v>22.0407325</v>
       </c>
     </row>
     <row r="76">
       <c r="A76" t="inlineStr">
         <is>
-          <t>United States</t>
+          <t>Colombia</t>
         </is>
       </c>
       <c r="B76" t="inlineStr">
         <is>
-          <t>USA</t>
+          <t>COL</t>
         </is>
       </c>
       <c r="C76" t="inlineStr">
         <is>
-          <t>Renew</t>
+          <t>PM</t>
         </is>
       </c>
       <c r="D76" t="inlineStr">
@@ -2250,23 +2250,23 @@
         </is>
       </c>
       <c r="E76">
-        <v>10.12</v>
+        <v>22.11926649</v>
       </c>
     </row>
     <row r="77">
       <c r="A77" t="inlineStr">
         <is>
-          <t>United States</t>
+          <t>Colombia</t>
         </is>
       </c>
       <c r="B77" t="inlineStr">
         <is>
-          <t>USA</t>
+          <t>COL</t>
         </is>
       </c>
       <c r="C77" t="inlineStr">
         <is>
-          <t>Renew</t>
+          <t>PM</t>
         </is>
       </c>
       <c r="D77" t="inlineStr">
@@ -2275,48 +2275,45 @@
         </is>
       </c>
       <c r="E77">
-        <v>10.42</v>
+        <v>22.01072747</v>
       </c>
     </row>
     <row r="78">
       <c r="A78" t="inlineStr">
         <is>
-          <t>United States</t>
+          <t>Colombia</t>
         </is>
       </c>
       <c r="B78" t="inlineStr">
         <is>
-          <t>USA</t>
+          <t>COL</t>
         </is>
       </c>
       <c r="C78" t="inlineStr">
         <is>
-          <t>Renew</t>
+          <t>PM</t>
         </is>
       </c>
       <c r="D78" t="inlineStr">
         <is>
           <t>2020</t>
         </is>
-      </c>
-      <c r="E78">
-        <v>11.16</v>
       </c>
     </row>
     <row r="79">
       <c r="A79" t="inlineStr">
         <is>
-          <t>United States</t>
+          <t>Colombia</t>
         </is>
       </c>
       <c r="B79" t="inlineStr">
         <is>
-          <t>USA</t>
+          <t>COL</t>
         </is>
       </c>
       <c r="C79" t="inlineStr">
         <is>
-          <t>Cook</t>
+          <t>CO2</t>
         </is>
       </c>
       <c r="D79" t="inlineStr">
@@ -2325,23 +2322,23 @@
         </is>
       </c>
       <c r="E79">
-        <v>100</v>
+        <v>1.43131795380357</v>
       </c>
     </row>
     <row r="80">
       <c r="A80" t="inlineStr">
         <is>
-          <t>United States</t>
+          <t>Colombia</t>
         </is>
       </c>
       <c r="B80" t="inlineStr">
         <is>
-          <t>USA</t>
+          <t>COL</t>
         </is>
       </c>
       <c r="C80" t="inlineStr">
         <is>
-          <t>Cook</t>
+          <t>CO2</t>
         </is>
       </c>
       <c r="D80" t="inlineStr">
@@ -2350,23 +2347,23 @@
         </is>
       </c>
       <c r="E80">
-        <v>100</v>
+        <v>1.53989837625496</v>
       </c>
     </row>
     <row r="81">
       <c r="A81" t="inlineStr">
         <is>
-          <t>United States</t>
+          <t>Colombia</t>
         </is>
       </c>
       <c r="B81" t="inlineStr">
         <is>
-          <t>USA</t>
+          <t>COL</t>
         </is>
       </c>
       <c r="C81" t="inlineStr">
         <is>
-          <t>Cook</t>
+          <t>CO2</t>
         </is>
       </c>
       <c r="D81" t="inlineStr">
@@ -2375,23 +2372,23 @@
         </is>
       </c>
       <c r="E81">
-        <v>100</v>
+        <v>1.53384649831834</v>
       </c>
     </row>
     <row r="82">
       <c r="A82" t="inlineStr">
         <is>
-          <t>United States</t>
+          <t>Colombia</t>
         </is>
       </c>
       <c r="B82" t="inlineStr">
         <is>
-          <t>USA</t>
+          <t>COL</t>
         </is>
       </c>
       <c r="C82" t="inlineStr">
         <is>
-          <t>Cook</t>
+          <t>CO2</t>
         </is>
       </c>
       <c r="D82" t="inlineStr">
@@ -2400,23 +2397,23 @@
         </is>
       </c>
       <c r="E82">
-        <v>100</v>
+        <v>1.68098788159418</v>
       </c>
     </row>
     <row r="83">
       <c r="A83" t="inlineStr">
         <is>
-          <t>United States</t>
+          <t>Colombia</t>
         </is>
       </c>
       <c r="B83" t="inlineStr">
         <is>
-          <t>USA</t>
+          <t>COL</t>
         </is>
       </c>
       <c r="C83" t="inlineStr">
         <is>
-          <t>Cook</t>
+          <t>CO2</t>
         </is>
       </c>
       <c r="D83" t="inlineStr">
@@ -2425,23 +2422,23 @@
         </is>
       </c>
       <c r="E83">
-        <v>100</v>
+        <v>1.71582096359122</v>
       </c>
     </row>
     <row r="84">
       <c r="A84" t="inlineStr">
         <is>
-          <t>United States</t>
+          <t>Colombia</t>
         </is>
       </c>
       <c r="B84" t="inlineStr">
         <is>
-          <t>USA</t>
+          <t>COL</t>
         </is>
       </c>
       <c r="C84" t="inlineStr">
         <is>
-          <t>Cook</t>
+          <t>CO2</t>
         </is>
       </c>
       <c r="D84" t="inlineStr">
@@ -2450,23 +2447,23 @@
         </is>
       </c>
       <c r="E84">
-        <v>100</v>
+        <v>1.71939023077553</v>
       </c>
     </row>
     <row r="85">
       <c r="A85" t="inlineStr">
         <is>
-          <t>United States</t>
+          <t>Colombia</t>
         </is>
       </c>
       <c r="B85" t="inlineStr">
         <is>
-          <t>USA</t>
+          <t>COL</t>
         </is>
       </c>
       <c r="C85" t="inlineStr">
         <is>
-          <t>Cook</t>
+          <t>CO2</t>
         </is>
       </c>
       <c r="D85" t="inlineStr">
@@ -2475,23 +2472,23 @@
         </is>
       </c>
       <c r="E85">
-        <v>100</v>
+        <v>1.75379580314977</v>
       </c>
     </row>
     <row r="86">
       <c r="A86" t="inlineStr">
         <is>
-          <t>United States</t>
+          <t>Colombia</t>
         </is>
       </c>
       <c r="B86" t="inlineStr">
         <is>
-          <t>USA</t>
+          <t>COL</t>
         </is>
       </c>
       <c r="C86" t="inlineStr">
         <is>
-          <t>Cook</t>
+          <t>CO2</t>
         </is>
       </c>
       <c r="D86" t="inlineStr">
@@ -2500,23 +2497,23 @@
         </is>
       </c>
       <c r="E86">
-        <v>100</v>
+        <v>1.56507517599547</v>
       </c>
     </row>
     <row r="87">
       <c r="A87" t="inlineStr">
         <is>
-          <t>United States</t>
+          <t>Colombia</t>
         </is>
       </c>
       <c r="B87" t="inlineStr">
         <is>
-          <t>USA</t>
+          <t>COL</t>
         </is>
       </c>
       <c r="C87" t="inlineStr">
         <is>
-          <t>Cook</t>
+          <t>CO2</t>
         </is>
       </c>
       <c r="D87" t="inlineStr">
@@ -2525,23 +2522,23 @@
         </is>
       </c>
       <c r="E87">
-        <v>100</v>
+        <v>1.61039151744768</v>
       </c>
     </row>
     <row r="88">
       <c r="A88" t="inlineStr">
         <is>
-          <t>United States</t>
+          <t>Colombia</t>
         </is>
       </c>
       <c r="B88" t="inlineStr">
         <is>
-          <t>USA</t>
+          <t>COL</t>
         </is>
       </c>
       <c r="C88" t="inlineStr">
         <is>
-          <t>Cook</t>
+          <t>CO2</t>
         </is>
       </c>
       <c r="D88" t="inlineStr">
@@ -2550,23 +2547,23 @@
         </is>
       </c>
       <c r="E88">
-        <v>100</v>
+        <v>1.57782014077396</v>
       </c>
     </row>
     <row r="89">
       <c r="A89" t="inlineStr">
         <is>
-          <t>United States</t>
+          <t>Colombia</t>
         </is>
       </c>
       <c r="B89" t="inlineStr">
         <is>
-          <t>USA</t>
+          <t>COL</t>
         </is>
       </c>
       <c r="C89" t="inlineStr">
         <is>
-          <t>Cook</t>
+          <t>CO2</t>
         </is>
       </c>
       <c r="D89" t="inlineStr">
@@ -2575,7 +2572,7 @@
         </is>
       </c>
       <c r="E89">
-        <v>100</v>
+        <v>1.552259422820776</v>
       </c>
     </row>
     <row r="90">
@@ -2591,7 +2588,7 @@
       </c>
       <c r="C90" t="inlineStr">
         <is>
-          <t>PM</t>
+          <t>Renew</t>
         </is>
       </c>
       <c r="D90" t="inlineStr">
@@ -2600,7 +2597,7 @@
         </is>
       </c>
       <c r="E90">
-        <v>25.0816067</v>
+        <v>29.63</v>
       </c>
     </row>
     <row r="91">
@@ -2616,7 +2613,7 @@
       </c>
       <c r="C91" t="inlineStr">
         <is>
-          <t>PM</t>
+          <t>Renew</t>
         </is>
       </c>
       <c r="D91" t="inlineStr">
@@ -2625,7 +2622,7 @@
         </is>
       </c>
       <c r="E91">
-        <v>25.94720366</v>
+        <v>28.74</v>
       </c>
     </row>
     <row r="92">
@@ -2641,7 +2638,7 @@
       </c>
       <c r="C92" t="inlineStr">
         <is>
-          <t>PM</t>
+          <t>Renew</t>
         </is>
       </c>
       <c r="D92" t="inlineStr">
@@ -2650,7 +2647,7 @@
         </is>
       </c>
       <c r="E92">
-        <v>23.4265212</v>
+        <v>28.8</v>
       </c>
     </row>
     <row r="93">
@@ -2666,7 +2663,7 @@
       </c>
       <c r="C93" t="inlineStr">
         <is>
-          <t>PM</t>
+          <t>Renew</t>
         </is>
       </c>
       <c r="D93" t="inlineStr">
@@ -2675,7 +2672,7 @@
         </is>
       </c>
       <c r="E93">
-        <v>24.2848162</v>
+        <v>32.13</v>
       </c>
     </row>
     <row r="94">
@@ -2691,7 +2688,7 @@
       </c>
       <c r="C94" t="inlineStr">
         <is>
-          <t>PM</t>
+          <t>Renew</t>
         </is>
       </c>
       <c r="D94" t="inlineStr">
@@ -2700,7 +2697,7 @@
         </is>
       </c>
       <c r="E94">
-        <v>23.85881131</v>
+        <v>32.22</v>
       </c>
     </row>
     <row r="95">
@@ -2716,7 +2713,7 @@
       </c>
       <c r="C95" t="inlineStr">
         <is>
-          <t>PM</t>
+          <t>Renew</t>
         </is>
       </c>
       <c r="D95" t="inlineStr">
@@ -2725,7 +2722,7 @@
         </is>
       </c>
       <c r="E95">
-        <v>22.92043409</v>
+        <v>31.46</v>
       </c>
     </row>
     <row r="96">
@@ -2741,7 +2738,7 @@
       </c>
       <c r="C96" t="inlineStr">
         <is>
-          <t>PM</t>
+          <t>Renew</t>
         </is>
       </c>
       <c r="D96" t="inlineStr">
@@ -2750,7 +2747,7 @@
         </is>
       </c>
       <c r="E96">
-        <v>22.72386043</v>
+        <v>30.6</v>
       </c>
     </row>
     <row r="97">
@@ -2766,7 +2763,7 @@
       </c>
       <c r="C97" t="inlineStr">
         <is>
-          <t>PM</t>
+          <t>Renew</t>
         </is>
       </c>
       <c r="D97" t="inlineStr">
@@ -2775,7 +2772,7 @@
         </is>
       </c>
       <c r="E97">
-        <v>22.0407325</v>
+        <v>32.38</v>
       </c>
     </row>
     <row r="98">
@@ -2791,7 +2788,7 @@
       </c>
       <c r="C98" t="inlineStr">
         <is>
-          <t>PM</t>
+          <t>Renew</t>
         </is>
       </c>
       <c r="D98" t="inlineStr">
@@ -2800,7 +2797,7 @@
         </is>
       </c>
       <c r="E98">
-        <v>22.11926649</v>
+        <v>30.57</v>
       </c>
     </row>
     <row r="99">
@@ -2816,7 +2813,7 @@
       </c>
       <c r="C99" t="inlineStr">
         <is>
-          <t>PM</t>
+          <t>Renew</t>
         </is>
       </c>
       <c r="D99" t="inlineStr">
@@ -2825,7 +2822,7 @@
         </is>
       </c>
       <c r="E99">
-        <v>22.01072747</v>
+        <v>31.5</v>
       </c>
     </row>
     <row r="100">
@@ -2841,29 +2838,32 @@
       </c>
       <c r="C100" t="inlineStr">
         <is>
-          <t>PM</t>
+          <t>Renew</t>
         </is>
       </c>
       <c r="D100" t="inlineStr">
         <is>
           <t>2020</t>
         </is>
+      </c>
+      <c r="E100">
+        <v>31.31</v>
       </c>
     </row>
     <row r="101">
       <c r="A101" t="inlineStr">
         <is>
-          <t>Colombia</t>
+          <t>Germany</t>
         </is>
       </c>
       <c r="B101" t="inlineStr">
         <is>
-          <t>COL</t>
+          <t>DEU</t>
         </is>
       </c>
       <c r="C101" t="inlineStr">
         <is>
-          <t>CO2</t>
+          <t>PM</t>
         </is>
       </c>
       <c r="D101" t="inlineStr">
@@ -2872,23 +2872,23 @@
         </is>
       </c>
       <c r="E101">
-        <v>1.43131795380357</v>
+        <v>16.08934354</v>
       </c>
     </row>
     <row r="102">
       <c r="A102" t="inlineStr">
         <is>
-          <t>Colombia</t>
+          <t>Germany</t>
         </is>
       </c>
       <c r="B102" t="inlineStr">
         <is>
-          <t>COL</t>
+          <t>DEU</t>
         </is>
       </c>
       <c r="C102" t="inlineStr">
         <is>
-          <t>CO2</t>
+          <t>PM</t>
         </is>
       </c>
       <c r="D102" t="inlineStr">
@@ -2897,23 +2897,23 @@
         </is>
       </c>
       <c r="E102">
-        <v>1.53989837625496</v>
+        <v>15.57511307</v>
       </c>
     </row>
     <row r="103">
       <c r="A103" t="inlineStr">
         <is>
-          <t>Colombia</t>
+          <t>Germany</t>
         </is>
       </c>
       <c r="B103" t="inlineStr">
         <is>
-          <t>COL</t>
+          <t>DEU</t>
         </is>
       </c>
       <c r="C103" t="inlineStr">
         <is>
-          <t>CO2</t>
+          <t>PM</t>
         </is>
       </c>
       <c r="D103" t="inlineStr">
@@ -2922,23 +2922,23 @@
         </is>
       </c>
       <c r="E103">
-        <v>1.53384649831834</v>
+        <v>13.8086903</v>
       </c>
     </row>
     <row r="104">
       <c r="A104" t="inlineStr">
         <is>
-          <t>Colombia</t>
+          <t>Germany</t>
         </is>
       </c>
       <c r="B104" t="inlineStr">
         <is>
-          <t>COL</t>
+          <t>DEU</t>
         </is>
       </c>
       <c r="C104" t="inlineStr">
         <is>
-          <t>CO2</t>
+          <t>PM</t>
         </is>
       </c>
       <c r="D104" t="inlineStr">
@@ -2947,23 +2947,23 @@
         </is>
       </c>
       <c r="E104">
-        <v>1.68098788159418</v>
+        <v>13.57835046</v>
       </c>
     </row>
     <row r="105">
       <c r="A105" t="inlineStr">
         <is>
-          <t>Colombia</t>
+          <t>Germany</t>
         </is>
       </c>
       <c r="B105" t="inlineStr">
         <is>
-          <t>COL</t>
+          <t>DEU</t>
         </is>
       </c>
       <c r="C105" t="inlineStr">
         <is>
-          <t>CO2</t>
+          <t>PM</t>
         </is>
       </c>
       <c r="D105" t="inlineStr">
@@ -2972,23 +2972,23 @@
         </is>
       </c>
       <c r="E105">
-        <v>1.71582096359122</v>
+        <v>12.24528447</v>
       </c>
     </row>
     <row r="106">
       <c r="A106" t="inlineStr">
         <is>
-          <t>Colombia</t>
+          <t>Germany</t>
         </is>
       </c>
       <c r="B106" t="inlineStr">
         <is>
-          <t>COL</t>
+          <t>DEU</t>
         </is>
       </c>
       <c r="C106" t="inlineStr">
         <is>
-          <t>CO2</t>
+          <t>PM</t>
         </is>
       </c>
       <c r="D106" t="inlineStr">
@@ -2997,23 +2997,23 @@
         </is>
       </c>
       <c r="E106">
-        <v>1.71939023077553</v>
+        <v>12.72693664</v>
       </c>
     </row>
     <row r="107">
       <c r="A107" t="inlineStr">
         <is>
-          <t>Colombia</t>
+          <t>Germany</t>
         </is>
       </c>
       <c r="B107" t="inlineStr">
         <is>
-          <t>COL</t>
+          <t>DEU</t>
         </is>
       </c>
       <c r="C107" t="inlineStr">
         <is>
-          <t>CO2</t>
+          <t>PM</t>
         </is>
       </c>
       <c r="D107" t="inlineStr">
@@ -3022,23 +3022,23 @@
         </is>
       </c>
       <c r="E107">
-        <v>1.75379580314977</v>
+        <v>11.77992518</v>
       </c>
     </row>
     <row r="108">
       <c r="A108" t="inlineStr">
         <is>
-          <t>Colombia</t>
+          <t>Germany</t>
         </is>
       </c>
       <c r="B108" t="inlineStr">
         <is>
-          <t>COL</t>
+          <t>DEU</t>
         </is>
       </c>
       <c r="C108" t="inlineStr">
         <is>
-          <t>CO2</t>
+          <t>PM</t>
         </is>
       </c>
       <c r="D108" t="inlineStr">
@@ -3047,23 +3047,23 @@
         </is>
       </c>
       <c r="E108">
-        <v>1.56507517599547</v>
+        <v>11.88161987</v>
       </c>
     </row>
     <row r="109">
       <c r="A109" t="inlineStr">
         <is>
-          <t>Colombia</t>
+          <t>Germany</t>
         </is>
       </c>
       <c r="B109" t="inlineStr">
         <is>
-          <t>COL</t>
+          <t>DEU</t>
         </is>
       </c>
       <c r="C109" t="inlineStr">
         <is>
-          <t>CO2</t>
+          <t>PM</t>
         </is>
       </c>
       <c r="D109" t="inlineStr">
@@ -3072,23 +3072,23 @@
         </is>
       </c>
       <c r="E109">
-        <v>1.61039151744768</v>
+        <v>11.92460308</v>
       </c>
     </row>
     <row r="110">
       <c r="A110" t="inlineStr">
         <is>
-          <t>Colombia</t>
+          <t>Germany</t>
         </is>
       </c>
       <c r="B110" t="inlineStr">
         <is>
-          <t>COL</t>
+          <t>DEU</t>
         </is>
       </c>
       <c r="C110" t="inlineStr">
         <is>
-          <t>CO2</t>
+          <t>PM</t>
         </is>
       </c>
       <c r="D110" t="inlineStr">
@@ -3097,48 +3097,45 @@
         </is>
       </c>
       <c r="E110">
-        <v>1.57782014077396</v>
+        <v>11.80580716</v>
       </c>
     </row>
     <row r="111">
       <c r="A111" t="inlineStr">
         <is>
-          <t>Colombia</t>
+          <t>Germany</t>
         </is>
       </c>
       <c r="B111" t="inlineStr">
         <is>
-          <t>COL</t>
+          <t>DEU</t>
         </is>
       </c>
       <c r="C111" t="inlineStr">
         <is>
-          <t>CO2</t>
+          <t>PM</t>
         </is>
       </c>
       <c r="D111" t="inlineStr">
         <is>
           <t>2020</t>
         </is>
-      </c>
-      <c r="E111">
-        <v>1.552259422820776</v>
       </c>
     </row>
     <row r="112">
       <c r="A112" t="inlineStr">
         <is>
-          <t>Colombia</t>
+          <t>Germany</t>
         </is>
       </c>
       <c r="B112" t="inlineStr">
         <is>
-          <t>COL</t>
+          <t>DEU</t>
         </is>
       </c>
       <c r="C112" t="inlineStr">
         <is>
-          <t>Renew</t>
+          <t>CO2</t>
         </is>
       </c>
       <c r="D112" t="inlineStr">
@@ -3147,23 +3144,23 @@
         </is>
       </c>
       <c r="E112">
-        <v>29.63</v>
+        <v>9.45338862684134</v>
       </c>
     </row>
     <row r="113">
       <c r="A113" t="inlineStr">
         <is>
-          <t>Colombia</t>
+          <t>Germany</t>
         </is>
       </c>
       <c r="B113" t="inlineStr">
         <is>
-          <t>COL</t>
+          <t>DEU</t>
         </is>
       </c>
       <c r="C113" t="inlineStr">
         <is>
-          <t>Renew</t>
+          <t>CO2</t>
         </is>
       </c>
       <c r="D113" t="inlineStr">
@@ -3172,23 +3169,23 @@
         </is>
       </c>
       <c r="E113">
-        <v>28.74</v>
+        <v>9.29900290355714</v>
       </c>
     </row>
     <row r="114">
       <c r="A114" t="inlineStr">
         <is>
-          <t>Colombia</t>
+          <t>Germany</t>
         </is>
       </c>
       <c r="B114" t="inlineStr">
         <is>
-          <t>COL</t>
+          <t>DEU</t>
         </is>
       </c>
       <c r="C114" t="inlineStr">
         <is>
-          <t>Renew</t>
+          <t>CO2</t>
         </is>
       </c>
       <c r="D114" t="inlineStr">
@@ -3197,23 +3194,23 @@
         </is>
       </c>
       <c r="E114">
-        <v>28.8</v>
+        <v>9.45128904680279</v>
       </c>
     </row>
     <row r="115">
       <c r="A115" t="inlineStr">
         <is>
-          <t>Colombia</t>
+          <t>Germany</t>
         </is>
       </c>
       <c r="B115" t="inlineStr">
         <is>
-          <t>COL</t>
+          <t>DEU</t>
         </is>
       </c>
       <c r="C115" t="inlineStr">
         <is>
-          <t>Renew</t>
+          <t>CO2</t>
         </is>
       </c>
       <c r="D115" t="inlineStr">
@@ -3222,23 +3219,23 @@
         </is>
       </c>
       <c r="E115">
-        <v>32.13</v>
+        <v>9.62422936749002</v>
       </c>
     </row>
     <row r="116">
       <c r="A116" t="inlineStr">
         <is>
-          <t>Colombia</t>
+          <t>Germany</t>
         </is>
       </c>
       <c r="B116" t="inlineStr">
         <is>
-          <t>COL</t>
+          <t>DEU</t>
         </is>
       </c>
       <c r="C116" t="inlineStr">
         <is>
-          <t>Renew</t>
+          <t>CO2</t>
         </is>
       </c>
       <c r="D116" t="inlineStr">
@@ -3247,23 +3244,23 @@
         </is>
       </c>
       <c r="E116">
-        <v>32.22</v>
+        <v>9.08852776834501</v>
       </c>
     </row>
     <row r="117">
       <c r="A117" t="inlineStr">
         <is>
-          <t>Colombia</t>
+          <t>Germany</t>
         </is>
       </c>
       <c r="B117" t="inlineStr">
         <is>
-          <t>COL</t>
+          <t>DEU</t>
         </is>
       </c>
       <c r="C117" t="inlineStr">
         <is>
-          <t>Renew</t>
+          <t>CO2</t>
         </is>
       </c>
       <c r="D117" t="inlineStr">
@@ -3272,23 +3269,23 @@
         </is>
       </c>
       <c r="E117">
-        <v>31.46</v>
+        <v>9.087344803666779</v>
       </c>
     </row>
     <row r="118">
       <c r="A118" t="inlineStr">
         <is>
-          <t>Colombia</t>
+          <t>Germany</t>
         </is>
       </c>
       <c r="B118" t="inlineStr">
         <is>
-          <t>COL</t>
+          <t>DEU</t>
         </is>
       </c>
       <c r="C118" t="inlineStr">
         <is>
-          <t>Renew</t>
+          <t>CO2</t>
         </is>
       </c>
       <c r="D118" t="inlineStr">
@@ -3297,23 +3294,23 @@
         </is>
       </c>
       <c r="E118">
-        <v>30.6</v>
+        <v>9.07297238768971</v>
       </c>
     </row>
     <row r="119">
       <c r="A119" t="inlineStr">
         <is>
-          <t>Colombia</t>
+          <t>Germany</t>
         </is>
       </c>
       <c r="B119" t="inlineStr">
         <is>
-          <t>COL</t>
+          <t>DEU</t>
         </is>
       </c>
       <c r="C119" t="inlineStr">
         <is>
-          <t>Renew</t>
+          <t>CO2</t>
         </is>
       </c>
       <c r="D119" t="inlineStr">
@@ -3322,23 +3319,23 @@
         </is>
       </c>
       <c r="E119">
-        <v>32.38</v>
+        <v>8.8583445114547</v>
       </c>
     </row>
     <row r="120">
       <c r="A120" t="inlineStr">
         <is>
-          <t>Colombia</t>
+          <t>Germany</t>
         </is>
       </c>
       <c r="B120" t="inlineStr">
         <is>
-          <t>COL</t>
+          <t>DEU</t>
         </is>
       </c>
       <c r="C120" t="inlineStr">
         <is>
-          <t>Renew</t>
+          <t>CO2</t>
         </is>
       </c>
       <c r="D120" t="inlineStr">
@@ -3347,23 +3344,23 @@
         </is>
       </c>
       <c r="E120">
-        <v>30.57</v>
+        <v>8.537042687806739</v>
       </c>
     </row>
     <row r="121">
       <c r="A121" t="inlineStr">
         <is>
-          <t>Colombia</t>
+          <t>Germany</t>
         </is>
       </c>
       <c r="B121" t="inlineStr">
         <is>
-          <t>COL</t>
+          <t>DEU</t>
         </is>
       </c>
       <c r="C121" t="inlineStr">
         <is>
-          <t>Renew</t>
+          <t>CO2</t>
         </is>
       </c>
       <c r="D121" t="inlineStr">
@@ -3372,23 +3369,23 @@
         </is>
       </c>
       <c r="E121">
-        <v>31.5</v>
+        <v>7.9271876239049</v>
       </c>
     </row>
     <row r="122">
       <c r="A122" t="inlineStr">
         <is>
-          <t>Colombia</t>
+          <t>Germany</t>
         </is>
       </c>
       <c r="B122" t="inlineStr">
         <is>
-          <t>COL</t>
+          <t>DEU</t>
         </is>
       </c>
       <c r="C122" t="inlineStr">
         <is>
-          <t>Renew</t>
+          <t>CO2</t>
         </is>
       </c>
       <c r="D122" t="inlineStr">
@@ -3397,23 +3394,23 @@
         </is>
       </c>
       <c r="E122">
-        <v>31.31</v>
+        <v>7.255221028168403</v>
       </c>
     </row>
     <row r="123">
       <c r="A123" t="inlineStr">
         <is>
-          <t>Colombia</t>
+          <t>Germany</t>
         </is>
       </c>
       <c r="B123" t="inlineStr">
         <is>
-          <t>COL</t>
+          <t>DEU</t>
         </is>
       </c>
       <c r="C123" t="inlineStr">
         <is>
-          <t>Cook</t>
+          <t>Renew</t>
         </is>
       </c>
       <c r="D123" t="inlineStr">
@@ -3422,23 +3419,23 @@
         </is>
       </c>
       <c r="E123">
-        <v>85.90000000000001</v>
+        <v>11.61</v>
       </c>
     </row>
     <row r="124">
       <c r="A124" t="inlineStr">
         <is>
-          <t>Colombia</t>
+          <t>Germany</t>
         </is>
       </c>
       <c r="B124" t="inlineStr">
         <is>
-          <t>COL</t>
+          <t>DEU</t>
         </is>
       </c>
       <c r="C124" t="inlineStr">
         <is>
-          <t>Cook</t>
+          <t>Renew</t>
         </is>
       </c>
       <c r="D124" t="inlineStr">
@@ -3447,23 +3444,23 @@
         </is>
       </c>
       <c r="E124">
-        <v>86.7</v>
+        <v>12.54</v>
       </c>
     </row>
     <row r="125">
       <c r="A125" t="inlineStr">
         <is>
-          <t>Colombia</t>
+          <t>Germany</t>
         </is>
       </c>
       <c r="B125" t="inlineStr">
         <is>
-          <t>COL</t>
+          <t>DEU</t>
         </is>
       </c>
       <c r="C125" t="inlineStr">
         <is>
-          <t>Cook</t>
+          <t>Renew</t>
         </is>
       </c>
       <c r="D125" t="inlineStr">
@@ -3472,23 +3469,23 @@
         </is>
       </c>
       <c r="E125">
-        <v>87.40000000000001</v>
+        <v>13.64</v>
       </c>
     </row>
     <row r="126">
       <c r="A126" t="inlineStr">
         <is>
-          <t>Colombia</t>
+          <t>Germany</t>
         </is>
       </c>
       <c r="B126" t="inlineStr">
         <is>
-          <t>COL</t>
+          <t>DEU</t>
         </is>
       </c>
       <c r="C126" t="inlineStr">
         <is>
-          <t>Cook</t>
+          <t>Renew</t>
         </is>
       </c>
       <c r="D126" t="inlineStr">
@@ -3497,23 +3494,23 @@
         </is>
       </c>
       <c r="E126">
-        <v>88.2</v>
+        <v>13.63</v>
       </c>
     </row>
     <row r="127">
       <c r="A127" t="inlineStr">
         <is>
-          <t>Colombia</t>
+          <t>Germany</t>
         </is>
       </c>
       <c r="B127" t="inlineStr">
         <is>
-          <t>COL</t>
+          <t>DEU</t>
         </is>
       </c>
       <c r="C127" t="inlineStr">
         <is>
-          <t>Cook</t>
+          <t>Renew</t>
         </is>
       </c>
       <c r="D127" t="inlineStr">
@@ -3522,23 +3519,23 @@
         </is>
       </c>
       <c r="E127">
-        <v>89</v>
+        <v>14.02</v>
       </c>
     </row>
     <row r="128">
       <c r="A128" t="inlineStr">
         <is>
-          <t>Colombia</t>
+          <t>Germany</t>
         </is>
       </c>
       <c r="B128" t="inlineStr">
         <is>
-          <t>COL</t>
+          <t>DEU</t>
         </is>
       </c>
       <c r="C128" t="inlineStr">
         <is>
-          <t>Cook</t>
+          <t>Renew</t>
         </is>
       </c>
       <c r="D128" t="inlineStr">
@@ -3547,23 +3544,23 @@
         </is>
       </c>
       <c r="E128">
-        <v>89.59999999999999</v>
+        <v>14.55</v>
       </c>
     </row>
     <row r="129">
       <c r="A129" t="inlineStr">
         <is>
-          <t>Colombia</t>
+          <t>Germany</t>
         </is>
       </c>
       <c r="B129" t="inlineStr">
         <is>
-          <t>COL</t>
+          <t>DEU</t>
         </is>
       </c>
       <c r="C129" t="inlineStr">
         <is>
-          <t>Cook</t>
+          <t>Renew</t>
         </is>
       </c>
       <c r="D129" t="inlineStr">
@@ -3572,23 +3569,23 @@
         </is>
       </c>
       <c r="E129">
-        <v>90.3</v>
+        <v>14.24</v>
       </c>
     </row>
     <row r="130">
       <c r="A130" t="inlineStr">
         <is>
-          <t>Colombia</t>
+          <t>Germany</t>
         </is>
       </c>
       <c r="B130" t="inlineStr">
         <is>
-          <t>COL</t>
+          <t>DEU</t>
         </is>
       </c>
       <c r="C130" t="inlineStr">
         <is>
-          <t>Cook</t>
+          <t>Renew</t>
         </is>
       </c>
       <c r="D130" t="inlineStr">
@@ -3597,23 +3594,23 @@
         </is>
       </c>
       <c r="E130">
-        <v>90.90000000000001</v>
+        <v>15.22</v>
       </c>
     </row>
     <row r="131">
       <c r="A131" t="inlineStr">
         <is>
-          <t>Colombia</t>
+          <t>Germany</t>
         </is>
       </c>
       <c r="B131" t="inlineStr">
         <is>
-          <t>COL</t>
+          <t>DEU</t>
         </is>
       </c>
       <c r="C131" t="inlineStr">
         <is>
-          <t>Cook</t>
+          <t>Renew</t>
         </is>
       </c>
       <c r="D131" t="inlineStr">
@@ -3622,23 +3619,23 @@
         </is>
       </c>
       <c r="E131">
-        <v>91.59999999999999</v>
+        <v>16.04</v>
       </c>
     </row>
     <row r="132">
       <c r="A132" t="inlineStr">
         <is>
-          <t>Colombia</t>
+          <t>Germany</t>
         </is>
       </c>
       <c r="B132" t="inlineStr">
         <is>
-          <t>COL</t>
+          <t>DEU</t>
         </is>
       </c>
       <c r="C132" t="inlineStr">
         <is>
-          <t>Cook</t>
+          <t>Renew</t>
         </is>
       </c>
       <c r="D132" t="inlineStr">
@@ -3647,23 +3644,23 @@
         </is>
       </c>
       <c r="E132">
-        <v>92.09999999999999</v>
+        <v>17.07</v>
       </c>
     </row>
     <row r="133">
       <c r="A133" t="inlineStr">
         <is>
-          <t>Colombia</t>
+          <t>Germany</t>
         </is>
       </c>
       <c r="B133" t="inlineStr">
         <is>
-          <t>COL</t>
+          <t>DEU</t>
         </is>
       </c>
       <c r="C133" t="inlineStr">
         <is>
-          <t>Cook</t>
+          <t>Renew</t>
         </is>
       </c>
       <c r="D133" t="inlineStr">
@@ -3672,1104 +3669,7 @@
         </is>
       </c>
       <c r="E133">
-        <v>92.8</v>
-      </c>
-    </row>
-    <row r="134">
-      <c r="A134" t="inlineStr">
-        <is>
-          <t>Germany</t>
-        </is>
-      </c>
-      <c r="B134" t="inlineStr">
-        <is>
-          <t>DEU</t>
-        </is>
-      </c>
-      <c r="C134" t="inlineStr">
-        <is>
-          <t>PM</t>
-        </is>
-      </c>
-      <c r="D134" t="inlineStr">
-        <is>
-          <t>2010</t>
-        </is>
-      </c>
-      <c r="E134">
-        <v>16.08934354</v>
-      </c>
-    </row>
-    <row r="135">
-      <c r="A135" t="inlineStr">
-        <is>
-          <t>Germany</t>
-        </is>
-      </c>
-      <c r="B135" t="inlineStr">
-        <is>
-          <t>DEU</t>
-        </is>
-      </c>
-      <c r="C135" t="inlineStr">
-        <is>
-          <t>PM</t>
-        </is>
-      </c>
-      <c r="D135" t="inlineStr">
-        <is>
-          <t>2011</t>
-        </is>
-      </c>
-      <c r="E135">
-        <v>15.57511307</v>
-      </c>
-    </row>
-    <row r="136">
-      <c r="A136" t="inlineStr">
-        <is>
-          <t>Germany</t>
-        </is>
-      </c>
-      <c r="B136" t="inlineStr">
-        <is>
-          <t>DEU</t>
-        </is>
-      </c>
-      <c r="C136" t="inlineStr">
-        <is>
-          <t>PM</t>
-        </is>
-      </c>
-      <c r="D136" t="inlineStr">
-        <is>
-          <t>2012</t>
-        </is>
-      </c>
-      <c r="E136">
-        <v>13.8086903</v>
-      </c>
-    </row>
-    <row r="137">
-      <c r="A137" t="inlineStr">
-        <is>
-          <t>Germany</t>
-        </is>
-      </c>
-      <c r="B137" t="inlineStr">
-        <is>
-          <t>DEU</t>
-        </is>
-      </c>
-      <c r="C137" t="inlineStr">
-        <is>
-          <t>PM</t>
-        </is>
-      </c>
-      <c r="D137" t="inlineStr">
-        <is>
-          <t>2013</t>
-        </is>
-      </c>
-      <c r="E137">
-        <v>13.57835046</v>
-      </c>
-    </row>
-    <row r="138">
-      <c r="A138" t="inlineStr">
-        <is>
-          <t>Germany</t>
-        </is>
-      </c>
-      <c r="B138" t="inlineStr">
-        <is>
-          <t>DEU</t>
-        </is>
-      </c>
-      <c r="C138" t="inlineStr">
-        <is>
-          <t>PM</t>
-        </is>
-      </c>
-      <c r="D138" t="inlineStr">
-        <is>
-          <t>2014</t>
-        </is>
-      </c>
-      <c r="E138">
-        <v>12.24528447</v>
-      </c>
-    </row>
-    <row r="139">
-      <c r="A139" t="inlineStr">
-        <is>
-          <t>Germany</t>
-        </is>
-      </c>
-      <c r="B139" t="inlineStr">
-        <is>
-          <t>DEU</t>
-        </is>
-      </c>
-      <c r="C139" t="inlineStr">
-        <is>
-          <t>PM</t>
-        </is>
-      </c>
-      <c r="D139" t="inlineStr">
-        <is>
-          <t>2015</t>
-        </is>
-      </c>
-      <c r="E139">
-        <v>12.72693664</v>
-      </c>
-    </row>
-    <row r="140">
-      <c r="A140" t="inlineStr">
-        <is>
-          <t>Germany</t>
-        </is>
-      </c>
-      <c r="B140" t="inlineStr">
-        <is>
-          <t>DEU</t>
-        </is>
-      </c>
-      <c r="C140" t="inlineStr">
-        <is>
-          <t>PM</t>
-        </is>
-      </c>
-      <c r="D140" t="inlineStr">
-        <is>
-          <t>2016</t>
-        </is>
-      </c>
-      <c r="E140">
-        <v>11.77992518</v>
-      </c>
-    </row>
-    <row r="141">
-      <c r="A141" t="inlineStr">
-        <is>
-          <t>Germany</t>
-        </is>
-      </c>
-      <c r="B141" t="inlineStr">
-        <is>
-          <t>DEU</t>
-        </is>
-      </c>
-      <c r="C141" t="inlineStr">
-        <is>
-          <t>PM</t>
-        </is>
-      </c>
-      <c r="D141" t="inlineStr">
-        <is>
-          <t>2017</t>
-        </is>
-      </c>
-      <c r="E141">
-        <v>11.88161987</v>
-      </c>
-    </row>
-    <row r="142">
-      <c r="A142" t="inlineStr">
-        <is>
-          <t>Germany</t>
-        </is>
-      </c>
-      <c r="B142" t="inlineStr">
-        <is>
-          <t>DEU</t>
-        </is>
-      </c>
-      <c r="C142" t="inlineStr">
-        <is>
-          <t>PM</t>
-        </is>
-      </c>
-      <c r="D142" t="inlineStr">
-        <is>
-          <t>2018</t>
-        </is>
-      </c>
-      <c r="E142">
-        <v>11.92460308</v>
-      </c>
-    </row>
-    <row r="143">
-      <c r="A143" t="inlineStr">
-        <is>
-          <t>Germany</t>
-        </is>
-      </c>
-      <c r="B143" t="inlineStr">
-        <is>
-          <t>DEU</t>
-        </is>
-      </c>
-      <c r="C143" t="inlineStr">
-        <is>
-          <t>PM</t>
-        </is>
-      </c>
-      <c r="D143" t="inlineStr">
-        <is>
-          <t>2019</t>
-        </is>
-      </c>
-      <c r="E143">
-        <v>11.80580716</v>
-      </c>
-    </row>
-    <row r="144">
-      <c r="A144" t="inlineStr">
-        <is>
-          <t>Germany</t>
-        </is>
-      </c>
-      <c r="B144" t="inlineStr">
-        <is>
-          <t>DEU</t>
-        </is>
-      </c>
-      <c r="C144" t="inlineStr">
-        <is>
-          <t>PM</t>
-        </is>
-      </c>
-      <c r="D144" t="inlineStr">
-        <is>
-          <t>2020</t>
-        </is>
-      </c>
-    </row>
-    <row r="145">
-      <c r="A145" t="inlineStr">
-        <is>
-          <t>Germany</t>
-        </is>
-      </c>
-      <c r="B145" t="inlineStr">
-        <is>
-          <t>DEU</t>
-        </is>
-      </c>
-      <c r="C145" t="inlineStr">
-        <is>
-          <t>CO2</t>
-        </is>
-      </c>
-      <c r="D145" t="inlineStr">
-        <is>
-          <t>2010</t>
-        </is>
-      </c>
-      <c r="E145">
-        <v>9.45338862684134</v>
-      </c>
-    </row>
-    <row r="146">
-      <c r="A146" t="inlineStr">
-        <is>
-          <t>Germany</t>
-        </is>
-      </c>
-      <c r="B146" t="inlineStr">
-        <is>
-          <t>DEU</t>
-        </is>
-      </c>
-      <c r="C146" t="inlineStr">
-        <is>
-          <t>CO2</t>
-        </is>
-      </c>
-      <c r="D146" t="inlineStr">
-        <is>
-          <t>2011</t>
-        </is>
-      </c>
-      <c r="E146">
-        <v>9.29900290355714</v>
-      </c>
-    </row>
-    <row r="147">
-      <c r="A147" t="inlineStr">
-        <is>
-          <t>Germany</t>
-        </is>
-      </c>
-      <c r="B147" t="inlineStr">
-        <is>
-          <t>DEU</t>
-        </is>
-      </c>
-      <c r="C147" t="inlineStr">
-        <is>
-          <t>CO2</t>
-        </is>
-      </c>
-      <c r="D147" t="inlineStr">
-        <is>
-          <t>2012</t>
-        </is>
-      </c>
-      <c r="E147">
-        <v>9.45128904680279</v>
-      </c>
-    </row>
-    <row r="148">
-      <c r="A148" t="inlineStr">
-        <is>
-          <t>Germany</t>
-        </is>
-      </c>
-      <c r="B148" t="inlineStr">
-        <is>
-          <t>DEU</t>
-        </is>
-      </c>
-      <c r="C148" t="inlineStr">
-        <is>
-          <t>CO2</t>
-        </is>
-      </c>
-      <c r="D148" t="inlineStr">
-        <is>
-          <t>2013</t>
-        </is>
-      </c>
-      <c r="E148">
-        <v>9.62422936749002</v>
-      </c>
-    </row>
-    <row r="149">
-      <c r="A149" t="inlineStr">
-        <is>
-          <t>Germany</t>
-        </is>
-      </c>
-      <c r="B149" t="inlineStr">
-        <is>
-          <t>DEU</t>
-        </is>
-      </c>
-      <c r="C149" t="inlineStr">
-        <is>
-          <t>CO2</t>
-        </is>
-      </c>
-      <c r="D149" t="inlineStr">
-        <is>
-          <t>2014</t>
-        </is>
-      </c>
-      <c r="E149">
-        <v>9.08852776834501</v>
-      </c>
-    </row>
-    <row r="150">
-      <c r="A150" t="inlineStr">
-        <is>
-          <t>Germany</t>
-        </is>
-      </c>
-      <c r="B150" t="inlineStr">
-        <is>
-          <t>DEU</t>
-        </is>
-      </c>
-      <c r="C150" t="inlineStr">
-        <is>
-          <t>CO2</t>
-        </is>
-      </c>
-      <c r="D150" t="inlineStr">
-        <is>
-          <t>2015</t>
-        </is>
-      </c>
-      <c r="E150">
-        <v>9.087344803666779</v>
-      </c>
-    </row>
-    <row r="151">
-      <c r="A151" t="inlineStr">
-        <is>
-          <t>Germany</t>
-        </is>
-      </c>
-      <c r="B151" t="inlineStr">
-        <is>
-          <t>DEU</t>
-        </is>
-      </c>
-      <c r="C151" t="inlineStr">
-        <is>
-          <t>CO2</t>
-        </is>
-      </c>
-      <c r="D151" t="inlineStr">
-        <is>
-          <t>2016</t>
-        </is>
-      </c>
-      <c r="E151">
-        <v>9.07297238768971</v>
-      </c>
-    </row>
-    <row r="152">
-      <c r="A152" t="inlineStr">
-        <is>
-          <t>Germany</t>
-        </is>
-      </c>
-      <c r="B152" t="inlineStr">
-        <is>
-          <t>DEU</t>
-        </is>
-      </c>
-      <c r="C152" t="inlineStr">
-        <is>
-          <t>CO2</t>
-        </is>
-      </c>
-      <c r="D152" t="inlineStr">
-        <is>
-          <t>2017</t>
-        </is>
-      </c>
-      <c r="E152">
-        <v>8.8583445114547</v>
-      </c>
-    </row>
-    <row r="153">
-      <c r="A153" t="inlineStr">
-        <is>
-          <t>Germany</t>
-        </is>
-      </c>
-      <c r="B153" t="inlineStr">
-        <is>
-          <t>DEU</t>
-        </is>
-      </c>
-      <c r="C153" t="inlineStr">
-        <is>
-          <t>CO2</t>
-        </is>
-      </c>
-      <c r="D153" t="inlineStr">
-        <is>
-          <t>2018</t>
-        </is>
-      </c>
-      <c r="E153">
-        <v>8.537042687806739</v>
-      </c>
-    </row>
-    <row r="154">
-      <c r="A154" t="inlineStr">
-        <is>
-          <t>Germany</t>
-        </is>
-      </c>
-      <c r="B154" t="inlineStr">
-        <is>
-          <t>DEU</t>
-        </is>
-      </c>
-      <c r="C154" t="inlineStr">
-        <is>
-          <t>CO2</t>
-        </is>
-      </c>
-      <c r="D154" t="inlineStr">
-        <is>
-          <t>2019</t>
-        </is>
-      </c>
-      <c r="E154">
-        <v>7.9271876239049</v>
-      </c>
-    </row>
-    <row r="155">
-      <c r="A155" t="inlineStr">
-        <is>
-          <t>Germany</t>
-        </is>
-      </c>
-      <c r="B155" t="inlineStr">
-        <is>
-          <t>DEU</t>
-        </is>
-      </c>
-      <c r="C155" t="inlineStr">
-        <is>
-          <t>CO2</t>
-        </is>
-      </c>
-      <c r="D155" t="inlineStr">
-        <is>
-          <t>2020</t>
-        </is>
-      </c>
-      <c r="E155">
-        <v>7.255221028168403</v>
-      </c>
-    </row>
-    <row r="156">
-      <c r="A156" t="inlineStr">
-        <is>
-          <t>Germany</t>
-        </is>
-      </c>
-      <c r="B156" t="inlineStr">
-        <is>
-          <t>DEU</t>
-        </is>
-      </c>
-      <c r="C156" t="inlineStr">
-        <is>
-          <t>Renew</t>
-        </is>
-      </c>
-      <c r="D156" t="inlineStr">
-        <is>
-          <t>2010</t>
-        </is>
-      </c>
-      <c r="E156">
-        <v>11.61</v>
-      </c>
-    </row>
-    <row r="157">
-      <c r="A157" t="inlineStr">
-        <is>
-          <t>Germany</t>
-        </is>
-      </c>
-      <c r="B157" t="inlineStr">
-        <is>
-          <t>DEU</t>
-        </is>
-      </c>
-      <c r="C157" t="inlineStr">
-        <is>
-          <t>Renew</t>
-        </is>
-      </c>
-      <c r="D157" t="inlineStr">
-        <is>
-          <t>2011</t>
-        </is>
-      </c>
-      <c r="E157">
-        <v>12.54</v>
-      </c>
-    </row>
-    <row r="158">
-      <c r="A158" t="inlineStr">
-        <is>
-          <t>Germany</t>
-        </is>
-      </c>
-      <c r="B158" t="inlineStr">
-        <is>
-          <t>DEU</t>
-        </is>
-      </c>
-      <c r="C158" t="inlineStr">
-        <is>
-          <t>Renew</t>
-        </is>
-      </c>
-      <c r="D158" t="inlineStr">
-        <is>
-          <t>2012</t>
-        </is>
-      </c>
-      <c r="E158">
-        <v>13.64</v>
-      </c>
-    </row>
-    <row r="159">
-      <c r="A159" t="inlineStr">
-        <is>
-          <t>Germany</t>
-        </is>
-      </c>
-      <c r="B159" t="inlineStr">
-        <is>
-          <t>DEU</t>
-        </is>
-      </c>
-      <c r="C159" t="inlineStr">
-        <is>
-          <t>Renew</t>
-        </is>
-      </c>
-      <c r="D159" t="inlineStr">
-        <is>
-          <t>2013</t>
-        </is>
-      </c>
-      <c r="E159">
-        <v>13.63</v>
-      </c>
-    </row>
-    <row r="160">
-      <c r="A160" t="inlineStr">
-        <is>
-          <t>Germany</t>
-        </is>
-      </c>
-      <c r="B160" t="inlineStr">
-        <is>
-          <t>DEU</t>
-        </is>
-      </c>
-      <c r="C160" t="inlineStr">
-        <is>
-          <t>Renew</t>
-        </is>
-      </c>
-      <c r="D160" t="inlineStr">
-        <is>
-          <t>2014</t>
-        </is>
-      </c>
-      <c r="E160">
-        <v>14.02</v>
-      </c>
-    </row>
-    <row r="161">
-      <c r="A161" t="inlineStr">
-        <is>
-          <t>Germany</t>
-        </is>
-      </c>
-      <c r="B161" t="inlineStr">
-        <is>
-          <t>DEU</t>
-        </is>
-      </c>
-      <c r="C161" t="inlineStr">
-        <is>
-          <t>Renew</t>
-        </is>
-      </c>
-      <c r="D161" t="inlineStr">
-        <is>
-          <t>2015</t>
-        </is>
-      </c>
-      <c r="E161">
-        <v>14.55</v>
-      </c>
-    </row>
-    <row r="162">
-      <c r="A162" t="inlineStr">
-        <is>
-          <t>Germany</t>
-        </is>
-      </c>
-      <c r="B162" t="inlineStr">
-        <is>
-          <t>DEU</t>
-        </is>
-      </c>
-      <c r="C162" t="inlineStr">
-        <is>
-          <t>Renew</t>
-        </is>
-      </c>
-      <c r="D162" t="inlineStr">
-        <is>
-          <t>2016</t>
-        </is>
-      </c>
-      <c r="E162">
-        <v>14.24</v>
-      </c>
-    </row>
-    <row r="163">
-      <c r="A163" t="inlineStr">
-        <is>
-          <t>Germany</t>
-        </is>
-      </c>
-      <c r="B163" t="inlineStr">
-        <is>
-          <t>DEU</t>
-        </is>
-      </c>
-      <c r="C163" t="inlineStr">
-        <is>
-          <t>Renew</t>
-        </is>
-      </c>
-      <c r="D163" t="inlineStr">
-        <is>
-          <t>2017</t>
-        </is>
-      </c>
-      <c r="E163">
-        <v>15.22</v>
-      </c>
-    </row>
-    <row r="164">
-      <c r="A164" t="inlineStr">
-        <is>
-          <t>Germany</t>
-        </is>
-      </c>
-      <c r="B164" t="inlineStr">
-        <is>
-          <t>DEU</t>
-        </is>
-      </c>
-      <c r="C164" t="inlineStr">
-        <is>
-          <t>Renew</t>
-        </is>
-      </c>
-      <c r="D164" t="inlineStr">
-        <is>
-          <t>2018</t>
-        </is>
-      </c>
-      <c r="E164">
-        <v>16.04</v>
-      </c>
-    </row>
-    <row r="165">
-      <c r="A165" t="inlineStr">
-        <is>
-          <t>Germany</t>
-        </is>
-      </c>
-      <c r="B165" t="inlineStr">
-        <is>
-          <t>DEU</t>
-        </is>
-      </c>
-      <c r="C165" t="inlineStr">
-        <is>
-          <t>Renew</t>
-        </is>
-      </c>
-      <c r="D165" t="inlineStr">
-        <is>
-          <t>2019</t>
-        </is>
-      </c>
-      <c r="E165">
-        <v>17.07</v>
-      </c>
-    </row>
-    <row r="166">
-      <c r="A166" t="inlineStr">
-        <is>
-          <t>Germany</t>
-        </is>
-      </c>
-      <c r="B166" t="inlineStr">
-        <is>
-          <t>DEU</t>
-        </is>
-      </c>
-      <c r="C166" t="inlineStr">
-        <is>
-          <t>Renew</t>
-        </is>
-      </c>
-      <c r="D166" t="inlineStr">
-        <is>
-          <t>2020</t>
-        </is>
-      </c>
-      <c r="E166">
         <v>18.6</v>
-      </c>
-    </row>
-    <row r="167">
-      <c r="A167" t="inlineStr">
-        <is>
-          <t>Germany</t>
-        </is>
-      </c>
-      <c r="B167" t="inlineStr">
-        <is>
-          <t>DEU</t>
-        </is>
-      </c>
-      <c r="C167" t="inlineStr">
-        <is>
-          <t>Cook</t>
-        </is>
-      </c>
-      <c r="D167" t="inlineStr">
-        <is>
-          <t>2010</t>
-        </is>
-      </c>
-      <c r="E167">
-        <v>100</v>
-      </c>
-    </row>
-    <row r="168">
-      <c r="A168" t="inlineStr">
-        <is>
-          <t>Germany</t>
-        </is>
-      </c>
-      <c r="B168" t="inlineStr">
-        <is>
-          <t>DEU</t>
-        </is>
-      </c>
-      <c r="C168" t="inlineStr">
-        <is>
-          <t>Cook</t>
-        </is>
-      </c>
-      <c r="D168" t="inlineStr">
-        <is>
-          <t>2011</t>
-        </is>
-      </c>
-      <c r="E168">
-        <v>100</v>
-      </c>
-    </row>
-    <row r="169">
-      <c r="A169" t="inlineStr">
-        <is>
-          <t>Germany</t>
-        </is>
-      </c>
-      <c r="B169" t="inlineStr">
-        <is>
-          <t>DEU</t>
-        </is>
-      </c>
-      <c r="C169" t="inlineStr">
-        <is>
-          <t>Cook</t>
-        </is>
-      </c>
-      <c r="D169" t="inlineStr">
-        <is>
-          <t>2012</t>
-        </is>
-      </c>
-      <c r="E169">
-        <v>100</v>
-      </c>
-    </row>
-    <row r="170">
-      <c r="A170" t="inlineStr">
-        <is>
-          <t>Germany</t>
-        </is>
-      </c>
-      <c r="B170" t="inlineStr">
-        <is>
-          <t>DEU</t>
-        </is>
-      </c>
-      <c r="C170" t="inlineStr">
-        <is>
-          <t>Cook</t>
-        </is>
-      </c>
-      <c r="D170" t="inlineStr">
-        <is>
-          <t>2013</t>
-        </is>
-      </c>
-      <c r="E170">
-        <v>100</v>
-      </c>
-    </row>
-    <row r="171">
-      <c r="A171" t="inlineStr">
-        <is>
-          <t>Germany</t>
-        </is>
-      </c>
-      <c r="B171" t="inlineStr">
-        <is>
-          <t>DEU</t>
-        </is>
-      </c>
-      <c r="C171" t="inlineStr">
-        <is>
-          <t>Cook</t>
-        </is>
-      </c>
-      <c r="D171" t="inlineStr">
-        <is>
-          <t>2014</t>
-        </is>
-      </c>
-      <c r="E171">
-        <v>100</v>
-      </c>
-    </row>
-    <row r="172">
-      <c r="A172" t="inlineStr">
-        <is>
-          <t>Germany</t>
-        </is>
-      </c>
-      <c r="B172" t="inlineStr">
-        <is>
-          <t>DEU</t>
-        </is>
-      </c>
-      <c r="C172" t="inlineStr">
-        <is>
-          <t>Cook</t>
-        </is>
-      </c>
-      <c r="D172" t="inlineStr">
-        <is>
-          <t>2015</t>
-        </is>
-      </c>
-      <c r="E172">
-        <v>100</v>
-      </c>
-    </row>
-    <row r="173">
-      <c r="A173" t="inlineStr">
-        <is>
-          <t>Germany</t>
-        </is>
-      </c>
-      <c r="B173" t="inlineStr">
-        <is>
-          <t>DEU</t>
-        </is>
-      </c>
-      <c r="C173" t="inlineStr">
-        <is>
-          <t>Cook</t>
-        </is>
-      </c>
-      <c r="D173" t="inlineStr">
-        <is>
-          <t>2016</t>
-        </is>
-      </c>
-      <c r="E173">
-        <v>100</v>
-      </c>
-    </row>
-    <row r="174">
-      <c r="A174" t="inlineStr">
-        <is>
-          <t>Germany</t>
-        </is>
-      </c>
-      <c r="B174" t="inlineStr">
-        <is>
-          <t>DEU</t>
-        </is>
-      </c>
-      <c r="C174" t="inlineStr">
-        <is>
-          <t>Cook</t>
-        </is>
-      </c>
-      <c r="D174" t="inlineStr">
-        <is>
-          <t>2017</t>
-        </is>
-      </c>
-      <c r="E174">
-        <v>100</v>
-      </c>
-    </row>
-    <row r="175">
-      <c r="A175" t="inlineStr">
-        <is>
-          <t>Germany</t>
-        </is>
-      </c>
-      <c r="B175" t="inlineStr">
-        <is>
-          <t>DEU</t>
-        </is>
-      </c>
-      <c r="C175" t="inlineStr">
-        <is>
-          <t>Cook</t>
-        </is>
-      </c>
-      <c r="D175" t="inlineStr">
-        <is>
-          <t>2018</t>
-        </is>
-      </c>
-      <c r="E175">
-        <v>100</v>
-      </c>
-    </row>
-    <row r="176">
-      <c r="A176" t="inlineStr">
-        <is>
-          <t>Germany</t>
-        </is>
-      </c>
-      <c r="B176" t="inlineStr">
-        <is>
-          <t>DEU</t>
-        </is>
-      </c>
-      <c r="C176" t="inlineStr">
-        <is>
-          <t>Cook</t>
-        </is>
-      </c>
-      <c r="D176" t="inlineStr">
-        <is>
-          <t>2019</t>
-        </is>
-      </c>
-      <c r="E176">
-        <v>100</v>
-      </c>
-    </row>
-    <row r="177">
-      <c r="A177" t="inlineStr">
-        <is>
-          <t>Germany</t>
-        </is>
-      </c>
-      <c r="B177" t="inlineStr">
-        <is>
-          <t>DEU</t>
-        </is>
-      </c>
-      <c r="C177" t="inlineStr">
-        <is>
-          <t>Cook</t>
-        </is>
-      </c>
-      <c r="D177" t="inlineStr">
-        <is>
-          <t>2020</t>
-        </is>
-      </c>
-      <c r="E177">
-        <v>100</v>
       </c>
     </row>
   </sheetData>

</xml_diff>